<commit_message>
Copy with over ride Facitly
</commit_message>
<xml_diff>
--- a/JsonToDVSDataLoader/src/main/java/com/gavs/automation/resources/MyHRTest.xlsx
+++ b/JsonToDVSDataLoader/src/main/java/com/gavs/automation/resources/MyHRTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="390" yWindow="645" windowWidth="19815" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
   <si>
     <t/>
   </si>
@@ -298,16 +298,40 @@
     <t>Alert</t>
   </si>
   <si>
-    <t>235</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>11</t>
+    <t>44</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>888</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>666</t>
   </si>
 </sst>
 </file>
@@ -771,6 +795,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2028825</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -835,6 +902,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="_xssf_cell_comment" hidden="1"/>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1274,7 +1384,7 @@
   <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:G9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1383,16 +1493,16 @@
         <v>0</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>